<commit_message>
add animal biology folks
</commit_message>
<xml_diff>
--- a/parsednames_checked.xlsx
+++ b/parsednames_checked.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/art/Documents/GitHub/nserc-pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2E1886-27DD-DE46-9A24-F4E6644569BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4323DAC4-37C8-524E-A11F-C64BA720FB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="23800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4446" uniqueCount="1921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5518" uniqueCount="2320">
   <si>
     <t>Program</t>
   </si>
@@ -5783,6 +5783,1203 @@
   </si>
   <si>
     <t>Laura Melissa Guzman Uribe</t>
+  </si>
+  <si>
+    <t>AnimalBio</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>Borowiec, BrittneyBG</t>
+  </si>
+  <si>
+    <t>BrittneyBG</t>
+  </si>
+  <si>
+    <t>Borowiec</t>
+  </si>
+  <si>
+    <t>Brittney B G</t>
+  </si>
+  <si>
+    <t>Brittney B G Borowiec</t>
+  </si>
+  <si>
+    <t>Gauberg, JuliaJ</t>
+  </si>
+  <si>
+    <t>JuliaJ</t>
+  </si>
+  <si>
+    <t>Gauberg</t>
+  </si>
+  <si>
+    <t>Julia J</t>
+  </si>
+  <si>
+    <t>Julia J Gauberg</t>
+  </si>
+  <si>
+    <t>Robertson, CayleihCEG</t>
+  </si>
+  <si>
+    <t>CayleihCEG</t>
+  </si>
+  <si>
+    <t>Cayleih C E G</t>
+  </si>
+  <si>
+    <t>Cayleih C E G Robertson</t>
+  </si>
+  <si>
+    <t>Salisbury, SarahSJ</t>
+  </si>
+  <si>
+    <t>SarahSJ</t>
+  </si>
+  <si>
+    <t>Salisbury</t>
+  </si>
+  <si>
+    <t>Sarah S J</t>
+  </si>
+  <si>
+    <t>Sarah S J Salisbury</t>
+  </si>
+  <si>
+    <t>Foris, Borbala</t>
+  </si>
+  <si>
+    <t>Borbala</t>
+  </si>
+  <si>
+    <t>Foris</t>
+  </si>
+  <si>
+    <t>Borbala Foris</t>
+  </si>
+  <si>
+    <t>Todd, Lauren</t>
+  </si>
+  <si>
+    <t>Lauren Todd</t>
+  </si>
+  <si>
+    <t>Birceanu, Oana</t>
+  </si>
+  <si>
+    <t>Oana</t>
+  </si>
+  <si>
+    <t>Birceanu</t>
+  </si>
+  <si>
+    <t>Oana Birceanu</t>
+  </si>
+  <si>
+    <t>Fouhse, Janelle</t>
+  </si>
+  <si>
+    <t>Fouhse</t>
+  </si>
+  <si>
+    <t>Janelle Fouhse</t>
+  </si>
+  <si>
+    <t>Pasternak, Jonathan</t>
+  </si>
+  <si>
+    <t>Pasternak</t>
+  </si>
+  <si>
+    <t>Jonathan Pasternak</t>
+  </si>
+  <si>
+    <t>Watt, Cortney</t>
+  </si>
+  <si>
+    <t>Cortney</t>
+  </si>
+  <si>
+    <t>Watt</t>
+  </si>
+  <si>
+    <t>Cortney Watt</t>
+  </si>
+  <si>
+    <t>Anstead, Clare</t>
+  </si>
+  <si>
+    <t>Anstead</t>
+  </si>
+  <si>
+    <t>Clare Anstead</t>
+  </si>
+  <si>
+    <t>Chin, EuniceHannah</t>
+  </si>
+  <si>
+    <t>EuniceHannah</t>
+  </si>
+  <si>
+    <t>Chin</t>
+  </si>
+  <si>
+    <t>Eunice Hannah</t>
+  </si>
+  <si>
+    <t>Eunice Hannah Chin</t>
+  </si>
+  <si>
+    <t>Guillot, Martin</t>
+  </si>
+  <si>
+    <t>Guillot</t>
+  </si>
+  <si>
+    <t>Martin Guillot</t>
+  </si>
+  <si>
+    <t>Schmidt, Kimberly</t>
+  </si>
+  <si>
+    <t>Kimberly</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>Kimberly Schmidt</t>
+  </si>
+  <si>
+    <t>Wood, Katharine</t>
+  </si>
+  <si>
+    <t>Katharine</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Katharine Wood</t>
+  </si>
+  <si>
+    <t>Gerson, Alexander</t>
+  </si>
+  <si>
+    <t>Gerson</t>
+  </si>
+  <si>
+    <t>Alexander Gerson</t>
+  </si>
+  <si>
+    <t>Woyengo, Tofuko</t>
+  </si>
+  <si>
+    <t>Tofuko</t>
+  </si>
+  <si>
+    <t>Woyengo</t>
+  </si>
+  <si>
+    <t>Tofuko Woyengo</t>
+  </si>
+  <si>
+    <t>Maddin, Hillary</t>
+  </si>
+  <si>
+    <t>Hillary</t>
+  </si>
+  <si>
+    <t>Maddin</t>
+  </si>
+  <si>
+    <t>Hillary Maddin</t>
+  </si>
+  <si>
+    <t>Careau, Vincent</t>
+  </si>
+  <si>
+    <t>Careau</t>
+  </si>
+  <si>
+    <t>Vincent Careau</t>
+  </si>
+  <si>
+    <t>McKinney, Melissa</t>
+  </si>
+  <si>
+    <t>McKinney</t>
+  </si>
+  <si>
+    <t>Mc-Kinney</t>
+  </si>
+  <si>
+    <t>Melissa McKinney</t>
+  </si>
+  <si>
+    <t>Newman, Amy</t>
+  </si>
+  <si>
+    <t>Newman</t>
+  </si>
+  <si>
+    <t>Amy Newman</t>
+  </si>
+  <si>
+    <t>Paluzzi, JeanPaul</t>
+  </si>
+  <si>
+    <t>JeanPaul</t>
+  </si>
+  <si>
+    <t>Paluzzi</t>
+  </si>
+  <si>
+    <t>Jean Paul</t>
+  </si>
+  <si>
+    <t>Jean Paul Paluzzi</t>
+  </si>
+  <si>
+    <t>Kent, Clément</t>
+  </si>
+  <si>
+    <t>Clément</t>
+  </si>
+  <si>
+    <t>Clément Kent</t>
+  </si>
+  <si>
+    <t>Nain, Sukhbir</t>
+  </si>
+  <si>
+    <t>Sukhbir</t>
+  </si>
+  <si>
+    <t>Nain</t>
+  </si>
+  <si>
+    <t>Sukhbir Nain</t>
+  </si>
+  <si>
+    <t>Arnot, Jon</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Arnot</t>
+  </si>
+  <si>
+    <t>Jon Arnot</t>
+  </si>
+  <si>
+    <t>Brown, Stephen</t>
+  </si>
+  <si>
+    <t>Stephen Brown</t>
+  </si>
+  <si>
+    <t>Fitzpatrick, John</t>
+  </si>
+  <si>
+    <t>Fitzpatrick</t>
+  </si>
+  <si>
+    <t>John Fitzpatrick</t>
+  </si>
+  <si>
+    <t>Paquin, Nicolas</t>
+  </si>
+  <si>
+    <t>Nicolas Paquin</t>
+  </si>
+  <si>
+    <t>Kamel, Stephanie</t>
+  </si>
+  <si>
+    <t>Kamel</t>
+  </si>
+  <si>
+    <t>Stephanie Kamel</t>
+  </si>
+  <si>
+    <t>Killen, Shaun</t>
+  </si>
+  <si>
+    <t>Shaun</t>
+  </si>
+  <si>
+    <t>Killen</t>
+  </si>
+  <si>
+    <t>Shaun Killen</t>
+  </si>
+  <si>
+    <t>Labbe, Normand</t>
+  </si>
+  <si>
+    <t>Normand</t>
+  </si>
+  <si>
+    <t>Labbe</t>
+  </si>
+  <si>
+    <t>Normand Labbe</t>
+  </si>
+  <si>
+    <t>Niel, Lee</t>
+  </si>
+  <si>
+    <t>Niel</t>
+  </si>
+  <si>
+    <t>Lee Niel</t>
+  </si>
+  <si>
+    <t>Sasseville, Maxime</t>
+  </si>
+  <si>
+    <t>Maxime</t>
+  </si>
+  <si>
+    <t>Sasseville</t>
+  </si>
+  <si>
+    <t>Maxime Sasseville</t>
+  </si>
+  <si>
+    <t>Basu, Niladri</t>
+  </si>
+  <si>
+    <t>Niladri</t>
+  </si>
+  <si>
+    <t>Basu</t>
+  </si>
+  <si>
+    <t>Niladri Basu</t>
+  </si>
+  <si>
+    <t>Becker, Joy</t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>Becker</t>
+  </si>
+  <si>
+    <t>Joy Becker</t>
+  </si>
+  <si>
+    <t>Cutler, Christopher</t>
+  </si>
+  <si>
+    <t>Cutler</t>
+  </si>
+  <si>
+    <t>Christopher Cutler</t>
+  </si>
+  <si>
+    <t>Hogan(Gallant), Natacha</t>
+  </si>
+  <si>
+    <t>Natacha</t>
+  </si>
+  <si>
+    <t>Hogan(Gallant)</t>
+  </si>
+  <si>
+    <t>Hogan(-Gallant)</t>
+  </si>
+  <si>
+    <t>Natacha Hogan</t>
+  </si>
+  <si>
+    <t>Morrissey, Christy</t>
+  </si>
+  <si>
+    <t>Christy</t>
+  </si>
+  <si>
+    <t>Morrissey</t>
+  </si>
+  <si>
+    <t>Christy Morrissey</t>
+  </si>
+  <si>
+    <t>Cooper, David</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>David Cooper</t>
+  </si>
+  <si>
+    <t>Mattila, Heather</t>
+  </si>
+  <si>
+    <t>Mattila</t>
+  </si>
+  <si>
+    <t>Heather Mattila</t>
+  </si>
+  <si>
+    <t>Darveau, CharlesAntoine</t>
+  </si>
+  <si>
+    <t>CharlesAntoine</t>
+  </si>
+  <si>
+    <t>Darveau</t>
+  </si>
+  <si>
+    <t>Charles Antoine</t>
+  </si>
+  <si>
+    <t>Charles Antoine Darveau</t>
+  </si>
+  <si>
+    <t>Duggavathi, Rajesha</t>
+  </si>
+  <si>
+    <t>Rajesha</t>
+  </si>
+  <si>
+    <t>Duggavathi</t>
+  </si>
+  <si>
+    <t>Rajesha Duggavathi</t>
+  </si>
+  <si>
+    <t>Paquin, Pierre</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Pierre Paquin</t>
+  </si>
+  <si>
+    <t>Pitcher, Trevor</t>
+  </si>
+  <si>
+    <t>Pitcher</t>
+  </si>
+  <si>
+    <t>Trevor Pitcher</t>
+  </si>
+  <si>
+    <t>Wootton, Sarah</t>
+  </si>
+  <si>
+    <t>Wootton</t>
+  </si>
+  <si>
+    <t>Sarah Wootton</t>
+  </si>
+  <si>
+    <t>Clark, Julie</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Julie Clark</t>
+  </si>
+  <si>
+    <t>Donini, Andrew</t>
+  </si>
+  <si>
+    <t>Donini</t>
+  </si>
+  <si>
+    <t>Andrew Donini</t>
+  </si>
+  <si>
+    <t>Gray, Michelle</t>
+  </si>
+  <si>
+    <t>Michelle Gray</t>
+  </si>
+  <si>
+    <t>Kuang, Shihuan</t>
+  </si>
+  <si>
+    <t>Shihuan</t>
+  </si>
+  <si>
+    <t>Kuang</t>
+  </si>
+  <si>
+    <t>Shihuan Kuang</t>
+  </si>
+  <si>
+    <t>Willis, Craig</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Willis</t>
+  </si>
+  <si>
+    <t>Craig Willis</t>
+  </si>
+  <si>
+    <t>Cooke, Steven</t>
+  </si>
+  <si>
+    <t>Cooke</t>
+  </si>
+  <si>
+    <t>Steven Cooke</t>
+  </si>
+  <si>
+    <t>Ardelli, Bernadette</t>
+  </si>
+  <si>
+    <t>Bernadette</t>
+  </si>
+  <si>
+    <t>Ardelli</t>
+  </si>
+  <si>
+    <t>Bernadette Ardelli</t>
+  </si>
+  <si>
+    <t>Barclay, Jeff</t>
+  </si>
+  <si>
+    <t>Barclay</t>
+  </si>
+  <si>
+    <t>Jeff Barclay</t>
+  </si>
+  <si>
+    <t>Cameron, Christopher</t>
+  </si>
+  <si>
+    <t>Christopher Cameron</t>
+  </si>
+  <si>
+    <t>Humphries, Murray</t>
+  </si>
+  <si>
+    <t>Humphries</t>
+  </si>
+  <si>
+    <t>Murray Humphries</t>
+  </si>
+  <si>
+    <t>Koeberle, Paulo</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>Koeberle</t>
+  </si>
+  <si>
+    <t>Paulo Koeberle</t>
+  </si>
+  <si>
+    <t>Mechawar, Naguib</t>
+  </si>
+  <si>
+    <t>Naguib</t>
+  </si>
+  <si>
+    <t>Mechawar</t>
+  </si>
+  <si>
+    <t>Naguib Mechawar</t>
+  </si>
+  <si>
+    <t>Robert, Claude</t>
+  </si>
+  <si>
+    <t>Claude</t>
+  </si>
+  <si>
+    <t>Claude Robert</t>
+  </si>
+  <si>
+    <t>Watts, Jon</t>
+  </si>
+  <si>
+    <t>Watts</t>
+  </si>
+  <si>
+    <t>Jon Watts</t>
+  </si>
+  <si>
+    <t>Cabanac, Arnaud</t>
+  </si>
+  <si>
+    <t>Arnaud</t>
+  </si>
+  <si>
+    <t>Cabanac</t>
+  </si>
+  <si>
+    <t>Arnaud Cabanac</t>
+  </si>
+  <si>
+    <t>Griffin, Lisa</t>
+  </si>
+  <si>
+    <t>Griffin</t>
+  </si>
+  <si>
+    <t>Lisa Griffin</t>
+  </si>
+  <si>
+    <t>Larsson, Hans</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Larsson</t>
+  </si>
+  <si>
+    <t>Hans Larsson</t>
+  </si>
+  <si>
+    <t>ReyesMoreno, Carlos</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>ReyesMoreno</t>
+  </si>
+  <si>
+    <t>Reyes-Moreno</t>
+  </si>
+  <si>
+    <t>Carlos Reyes-Moreno</t>
+  </si>
+  <si>
+    <t>Gee, Christine</t>
+  </si>
+  <si>
+    <t>Gee</t>
+  </si>
+  <si>
+    <t>Christine Gee</t>
+  </si>
+  <si>
+    <t>Godfrey, Matthew</t>
+  </si>
+  <si>
+    <t>Godfrey</t>
+  </si>
+  <si>
+    <t>Matthew Godfrey</t>
+  </si>
+  <si>
+    <t>Bradshaw, Sheri</t>
+  </si>
+  <si>
+    <t>Sheri</t>
+  </si>
+  <si>
+    <t>Sheri Bradshaw</t>
+  </si>
+  <si>
+    <t>MacDougallShackleton, Scott</t>
+  </si>
+  <si>
+    <t>Scott MacDougall-Shackleton</t>
+  </si>
+  <si>
+    <t>Morrison, Sean</t>
+  </si>
+  <si>
+    <t>Morrison</t>
+  </si>
+  <si>
+    <t>Sean Morrison</t>
+  </si>
+  <si>
+    <t>Schofield, Steven</t>
+  </si>
+  <si>
+    <t>Schofield</t>
+  </si>
+  <si>
+    <t>Steven Schofield</t>
+  </si>
+  <si>
+    <t>vandeLavoir, MarieCecile</t>
+  </si>
+  <si>
+    <t>MarieCecile</t>
+  </si>
+  <si>
+    <t>vandeLavoir</t>
+  </si>
+  <si>
+    <t>Marie Cecile</t>
+  </si>
+  <si>
+    <t>Lavoir</t>
+  </si>
+  <si>
+    <t>Marie Cecile Lavoir</t>
+  </si>
+  <si>
+    <t>Ali, Declan</t>
+  </si>
+  <si>
+    <t>Declan</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Declan Ali</t>
+  </si>
+  <si>
+    <t>Pilon, Marc</t>
+  </si>
+  <si>
+    <t>Pilon</t>
+  </si>
+  <si>
+    <t>Marc Pilon</t>
+  </si>
+  <si>
+    <t>Zorn, Aaron</t>
+  </si>
+  <si>
+    <t>Zorn</t>
+  </si>
+  <si>
+    <t>Aaron Zorn</t>
+  </si>
+  <si>
+    <t>Bisgrove, Brent</t>
+  </si>
+  <si>
+    <t>Bisgrove</t>
+  </si>
+  <si>
+    <t>Brent Bisgrove</t>
+  </si>
+  <si>
+    <t>DeSousa, Paul</t>
+  </si>
+  <si>
+    <t>DeSousa</t>
+  </si>
+  <si>
+    <t>De-Sousa</t>
+  </si>
+  <si>
+    <t>Paul De-Sousa</t>
+  </si>
+  <si>
+    <t>Paul DeSousa</t>
+  </si>
+  <si>
+    <t>Krochko, Joan</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>Krochko</t>
+  </si>
+  <si>
+    <t>Joan Krochko</t>
+  </si>
+  <si>
+    <t>Leroi, Armand</t>
+  </si>
+  <si>
+    <t>Leroi</t>
+  </si>
+  <si>
+    <t>Armand Leroi</t>
+  </si>
+  <si>
+    <t>Lydan, Michael</t>
+  </si>
+  <si>
+    <t>Lydan</t>
+  </si>
+  <si>
+    <t>Michael Lydan</t>
+  </si>
+  <si>
+    <t>Telmer, Cheryl</t>
+  </si>
+  <si>
+    <t>Telmer</t>
+  </si>
+  <si>
+    <t>Cheryl Telmer</t>
+  </si>
+  <si>
+    <t>Bain, Gerard</t>
+  </si>
+  <si>
+    <t>Gerard</t>
+  </si>
+  <si>
+    <t>Bain</t>
+  </si>
+  <si>
+    <t>Gerard Bain</t>
+  </si>
+  <si>
+    <t>Moens, Cecilia</t>
+  </si>
+  <si>
+    <t>Cecilia</t>
+  </si>
+  <si>
+    <t>Moens</t>
+  </si>
+  <si>
+    <t>Cecilia Moens</t>
+  </si>
+  <si>
+    <t>Nachtigal, Mark</t>
+  </si>
+  <si>
+    <t>Nachtigal</t>
+  </si>
+  <si>
+    <t>Mark Nachtigal</t>
+  </si>
+  <si>
+    <t>Anholt, Bradley</t>
+  </si>
+  <si>
+    <t>Anholt</t>
+  </si>
+  <si>
+    <t>Bradley Anholt</t>
+  </si>
+  <si>
+    <t>Champagne, Donald</t>
+  </si>
+  <si>
+    <t>Champagne</t>
+  </si>
+  <si>
+    <t>Donald Champagne</t>
+  </si>
+  <si>
+    <t>Funk, Gregory</t>
+  </si>
+  <si>
+    <t>Funk</t>
+  </si>
+  <si>
+    <t>Gregory Funk</t>
+  </si>
+  <si>
+    <t>Smith, Steven</t>
+  </si>
+  <si>
+    <t>Steven Smith</t>
+  </si>
+  <si>
+    <t>Waas, Joseph</t>
+  </si>
+  <si>
+    <t>Waas</t>
+  </si>
+  <si>
+    <t>Joseph Waas</t>
+  </si>
+  <si>
+    <t>Whiteley, Mary</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Whiteley</t>
+  </si>
+  <si>
+    <t>Mary Whiteley</t>
+  </si>
+  <si>
+    <t>Adamo, Shelley</t>
+  </si>
+  <si>
+    <t>Adamo</t>
+  </si>
+  <si>
+    <t>Shelley Adamo</t>
+  </si>
+  <si>
+    <t>Boileau, Marc</t>
+  </si>
+  <si>
+    <t>Boileau</t>
+  </si>
+  <si>
+    <t>Marc Boileau</t>
+  </si>
+  <si>
+    <t>Bres, Odd</t>
+  </si>
+  <si>
+    <t>Odd</t>
+  </si>
+  <si>
+    <t>Bres</t>
+  </si>
+  <si>
+    <t>Odd Bres</t>
+  </si>
+  <si>
+    <t>Brown, Brian</t>
+  </si>
+  <si>
+    <t>Brian Brown</t>
+  </si>
+  <si>
+    <t>Bryant, Harold</t>
+  </si>
+  <si>
+    <t>Bryant</t>
+  </si>
+  <si>
+    <t>Harold Bryant</t>
+  </si>
+  <si>
+    <t>Cartar, Ralph</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Cartar</t>
+  </si>
+  <si>
+    <t>Ralph Cartar</t>
+  </si>
+  <si>
+    <t>Conn, Jan</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Conn</t>
+  </si>
+  <si>
+    <t>Jan Conn</t>
+  </si>
+  <si>
+    <t>Cooch, Evan</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t>Cooch</t>
+  </si>
+  <si>
+    <t>Evan Cooch</t>
+  </si>
+  <si>
+    <t>Cusson, Michel</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>Cusson</t>
+  </si>
+  <si>
+    <t>Michel Cusson</t>
+  </si>
+  <si>
+    <t>daSilva, Jack</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>daSilva</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Jack Silva</t>
+  </si>
+  <si>
+    <t>Dixon, Donald</t>
+  </si>
+  <si>
+    <t>Dixon</t>
+  </si>
+  <si>
+    <t>Donald Dixon</t>
+  </si>
+  <si>
+    <t>Ferguson, Ralph</t>
+  </si>
+  <si>
+    <t>Ferguson</t>
+  </si>
+  <si>
+    <t>Ralph Ferguson</t>
+  </si>
+  <si>
+    <t>Hudon, Jocelyn</t>
+  </si>
+  <si>
+    <t>Hudon</t>
+  </si>
+  <si>
+    <t>Jocelyn Hudon</t>
+  </si>
+  <si>
+    <t>Johnsen, Robert</t>
+  </si>
+  <si>
+    <t>Johnsen</t>
+  </si>
+  <si>
+    <t>Robert Johnsen</t>
+  </si>
+  <si>
+    <t>Lacoursière, Jean</t>
+  </si>
+  <si>
+    <t>Lacoursière</t>
+  </si>
+  <si>
+    <t>Jean Lacoursière</t>
+  </si>
+  <si>
+    <t>OFoighil, Diarmaid</t>
+  </si>
+  <si>
+    <t>Diarmaid</t>
+  </si>
+  <si>
+    <t>OFoighil</t>
+  </si>
+  <si>
+    <t>O-Foighil</t>
+  </si>
+  <si>
+    <t>Diarmaid OFoighil</t>
+  </si>
+  <si>
+    <t>Ovaska, Kristiina</t>
+  </si>
+  <si>
+    <t>Kristiina</t>
+  </si>
+  <si>
+    <t>Ovaska</t>
+  </si>
+  <si>
+    <t>Kristiina Ovaska</t>
+  </si>
+  <si>
+    <t>Playle, Richard</t>
+  </si>
+  <si>
+    <t>Playle</t>
+  </si>
+  <si>
+    <t>Richard Playle</t>
+  </si>
+  <si>
+    <t>Promislow, Daniel</t>
+  </si>
+  <si>
+    <t>Promislow</t>
+  </si>
+  <si>
+    <t>Daniel Promislow</t>
+  </si>
+  <si>
+    <t>Prusky, Glen</t>
+  </si>
+  <si>
+    <t>Glen</t>
+  </si>
+  <si>
+    <t>Prusky</t>
+  </si>
+  <si>
+    <t>Glen Prusky</t>
+  </si>
+  <si>
+    <t>Reynolds, John</t>
+  </si>
+  <si>
+    <t>Reynolds</t>
+  </si>
+  <si>
+    <t>John Reynolds</t>
+  </si>
+  <si>
+    <t>Richardson, John</t>
+  </si>
+  <si>
+    <t>John Richardson</t>
+  </si>
+  <si>
+    <t>Soluk, Daniel</t>
+  </si>
+  <si>
+    <t>Soluk</t>
+  </si>
+  <si>
+    <t>Daniel Soluk</t>
+  </si>
+  <si>
+    <t>Sukhdeo, Suzanne</t>
+  </si>
+  <si>
+    <t>Sukhdeo</t>
+  </si>
+  <si>
+    <t>Suzanne Sukhdeo</t>
+  </si>
+  <si>
+    <t>Taylor, Eric</t>
+  </si>
+  <si>
+    <t>Eric Taylor</t>
+  </si>
+  <si>
+    <t>Teather, Kevin</t>
+  </si>
+  <si>
+    <t>Teather</t>
+  </si>
+  <si>
+    <t>Kevin Teather</t>
+  </si>
+  <si>
+    <t>Thomson, Robert</t>
+  </si>
+  <si>
+    <t>Thomson</t>
+  </si>
+  <si>
+    <t>Robert Thomson</t>
   </si>
 </sst>
 </file>
@@ -6135,10 +7332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H582"/>
+  <dimension ref="A1:H716"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
-      <selection activeCell="B548" sqref="B548"/>
+    <sheetView tabSelected="1" topLeftCell="A665" workbookViewId="0">
+      <selection activeCell="K684" sqref="K684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20760,6 +21957,3490 @@
         <v>1920</v>
       </c>
     </row>
+    <row r="583" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C583" t="s">
+        <v>1923</v>
+      </c>
+      <c r="D583" t="s">
+        <v>1924</v>
+      </c>
+      <c r="E583" t="s">
+        <v>1925</v>
+      </c>
+      <c r="F583" t="s">
+        <v>1926</v>
+      </c>
+      <c r="G583" t="s">
+        <v>1925</v>
+      </c>
+      <c r="H583" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="584" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C584" t="s">
+        <v>1928</v>
+      </c>
+      <c r="D584" t="s">
+        <v>1929</v>
+      </c>
+      <c r="E584" t="s">
+        <v>1930</v>
+      </c>
+      <c r="F584" t="s">
+        <v>1931</v>
+      </c>
+      <c r="G584" t="s">
+        <v>1930</v>
+      </c>
+      <c r="H584" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="585" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B585" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C585" t="s">
+        <v>1933</v>
+      </c>
+      <c r="D585" t="s">
+        <v>1934</v>
+      </c>
+      <c r="E585" t="s">
+        <v>1480</v>
+      </c>
+      <c r="F585" t="s">
+        <v>1935</v>
+      </c>
+      <c r="G585" t="s">
+        <v>1480</v>
+      </c>
+      <c r="H585" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A586" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B586" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C586" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D586" t="s">
+        <v>1938</v>
+      </c>
+      <c r="E586" t="s">
+        <v>1939</v>
+      </c>
+      <c r="F586" t="s">
+        <v>1940</v>
+      </c>
+      <c r="G586" t="s">
+        <v>1939</v>
+      </c>
+      <c r="H586" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A587" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B587" t="s">
+        <v>9</v>
+      </c>
+      <c r="C587" t="s">
+        <v>1942</v>
+      </c>
+      <c r="D587" t="s">
+        <v>1943</v>
+      </c>
+      <c r="E587" t="s">
+        <v>1944</v>
+      </c>
+      <c r="F587" t="s">
+        <v>1943</v>
+      </c>
+      <c r="G587" t="s">
+        <v>1944</v>
+      </c>
+      <c r="H587" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="588" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A588" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B588" t="s">
+        <v>35</v>
+      </c>
+      <c r="C588" t="s">
+        <v>1946</v>
+      </c>
+      <c r="D588" t="s">
+        <v>109</v>
+      </c>
+      <c r="E588" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F588" t="s">
+        <v>109</v>
+      </c>
+      <c r="G588" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H588" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="589" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A589" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B589" t="s">
+        <v>70</v>
+      </c>
+      <c r="C589" t="s">
+        <v>1948</v>
+      </c>
+      <c r="D589" t="s">
+        <v>1949</v>
+      </c>
+      <c r="E589" t="s">
+        <v>1950</v>
+      </c>
+      <c r="F589" t="s">
+        <v>1949</v>
+      </c>
+      <c r="G589" t="s">
+        <v>1950</v>
+      </c>
+      <c r="H589" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="590" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B590" t="s">
+        <v>147</v>
+      </c>
+      <c r="C590" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D590" t="s">
+        <v>860</v>
+      </c>
+      <c r="E590" t="s">
+        <v>1953</v>
+      </c>
+      <c r="F590" t="s">
+        <v>860</v>
+      </c>
+      <c r="G590" t="s">
+        <v>1953</v>
+      </c>
+      <c r="H590" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B591" t="s">
+        <v>242</v>
+      </c>
+      <c r="C591" t="s">
+        <v>1955</v>
+      </c>
+      <c r="D591" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E591" t="s">
+        <v>1956</v>
+      </c>
+      <c r="F591" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G591" t="s">
+        <v>1956</v>
+      </c>
+      <c r="H591" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="592" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A592" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B592" t="s">
+        <v>242</v>
+      </c>
+      <c r="C592" t="s">
+        <v>1958</v>
+      </c>
+      <c r="D592" t="s">
+        <v>1959</v>
+      </c>
+      <c r="E592" t="s">
+        <v>1960</v>
+      </c>
+      <c r="F592" t="s">
+        <v>1959</v>
+      </c>
+      <c r="G592" t="s">
+        <v>1960</v>
+      </c>
+      <c r="H592" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="593" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A593" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B593" t="s">
+        <v>284</v>
+      </c>
+      <c r="C593" t="s">
+        <v>1962</v>
+      </c>
+      <c r="D593" t="s">
+        <v>459</v>
+      </c>
+      <c r="E593" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F593" t="s">
+        <v>459</v>
+      </c>
+      <c r="G593" t="s">
+        <v>1963</v>
+      </c>
+      <c r="H593" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="594" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A594" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B594" t="s">
+        <v>284</v>
+      </c>
+      <c r="C594" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D594" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E594" t="s">
+        <v>1967</v>
+      </c>
+      <c r="F594" t="s">
+        <v>1968</v>
+      </c>
+      <c r="G594" t="s">
+        <v>1967</v>
+      </c>
+      <c r="H594" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="595" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A595" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B595" t="s">
+        <v>284</v>
+      </c>
+      <c r="C595" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D595" t="s">
+        <v>264</v>
+      </c>
+      <c r="E595" t="s">
+        <v>1971</v>
+      </c>
+      <c r="F595" t="s">
+        <v>264</v>
+      </c>
+      <c r="G595" t="s">
+        <v>1971</v>
+      </c>
+      <c r="H595" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="596" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A596" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B596" t="s">
+        <v>284</v>
+      </c>
+      <c r="C596" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E596" t="s">
+        <v>1975</v>
+      </c>
+      <c r="F596" t="s">
+        <v>1974</v>
+      </c>
+      <c r="G596" t="s">
+        <v>1975</v>
+      </c>
+      <c r="H596" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="597" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A597" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B597" t="s">
+        <v>284</v>
+      </c>
+      <c r="C597" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E597" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F597" t="s">
+        <v>1978</v>
+      </c>
+      <c r="G597" t="s">
+        <v>1979</v>
+      </c>
+      <c r="H597" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="598" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A598" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B598" t="s">
+        <v>343</v>
+      </c>
+      <c r="C598" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D598" t="s">
+        <v>387</v>
+      </c>
+      <c r="E598" t="s">
+        <v>1982</v>
+      </c>
+      <c r="F598" t="s">
+        <v>387</v>
+      </c>
+      <c r="G598" t="s">
+        <v>1982</v>
+      </c>
+      <c r="H598" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="599" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A599" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B599" t="s">
+        <v>343</v>
+      </c>
+      <c r="C599" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D599" t="s">
+        <v>1985</v>
+      </c>
+      <c r="E599" t="s">
+        <v>1986</v>
+      </c>
+      <c r="F599" t="s">
+        <v>1985</v>
+      </c>
+      <c r="G599" t="s">
+        <v>1986</v>
+      </c>
+      <c r="H599" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="600" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A600" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B600" t="s">
+        <v>385</v>
+      </c>
+      <c r="C600" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D600" t="s">
+        <v>1989</v>
+      </c>
+      <c r="E600" t="s">
+        <v>1990</v>
+      </c>
+      <c r="F600" t="s">
+        <v>1989</v>
+      </c>
+      <c r="G600" t="s">
+        <v>1990</v>
+      </c>
+      <c r="H600" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="601" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A601" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B601" t="s">
+        <v>452</v>
+      </c>
+      <c r="C601" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D601" t="s">
+        <v>219</v>
+      </c>
+      <c r="E601" t="s">
+        <v>1993</v>
+      </c>
+      <c r="F601" t="s">
+        <v>219</v>
+      </c>
+      <c r="G601" t="s">
+        <v>1993</v>
+      </c>
+      <c r="H601" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="602" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A602" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B602" t="s">
+        <v>452</v>
+      </c>
+      <c r="C602" t="s">
+        <v>1995</v>
+      </c>
+      <c r="D602" t="s">
+        <v>135</v>
+      </c>
+      <c r="E602" t="s">
+        <v>1996</v>
+      </c>
+      <c r="F602" t="s">
+        <v>135</v>
+      </c>
+      <c r="G602" t="s">
+        <v>1997</v>
+      </c>
+      <c r="H602" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="603" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A603" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B603" t="s">
+        <v>452</v>
+      </c>
+      <c r="C603" t="s">
+        <v>1999</v>
+      </c>
+      <c r="D603" t="s">
+        <v>1793</v>
+      </c>
+      <c r="E603" t="s">
+        <v>2000</v>
+      </c>
+      <c r="F603" t="s">
+        <v>1793</v>
+      </c>
+      <c r="G603" t="s">
+        <v>2000</v>
+      </c>
+      <c r="H603" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="604" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A604" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B604" t="s">
+        <v>452</v>
+      </c>
+      <c r="C604" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D604" t="s">
+        <v>2003</v>
+      </c>
+      <c r="E604" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F604" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G604" t="s">
+        <v>2004</v>
+      </c>
+      <c r="H604" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="605" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A605" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B605" t="s">
+        <v>523</v>
+      </c>
+      <c r="C605" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D605" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E605" t="s">
+        <v>1339</v>
+      </c>
+      <c r="F605" t="s">
+        <v>2008</v>
+      </c>
+      <c r="G605" t="s">
+        <v>1339</v>
+      </c>
+      <c r="H605" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="606" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A606" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B606" t="s">
+        <v>523</v>
+      </c>
+      <c r="C606" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D606" t="s">
+        <v>2011</v>
+      </c>
+      <c r="E606" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F606" t="s">
+        <v>2011</v>
+      </c>
+      <c r="G606" t="s">
+        <v>2012</v>
+      </c>
+      <c r="H606" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="607" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A607" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B607" t="s">
+        <v>619</v>
+      </c>
+      <c r="C607" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D607" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E607" t="s">
+        <v>2016</v>
+      </c>
+      <c r="F607" t="s">
+        <v>2015</v>
+      </c>
+      <c r="G607" t="s">
+        <v>2016</v>
+      </c>
+      <c r="H607" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="608" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A608" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B608" t="s">
+        <v>619</v>
+      </c>
+      <c r="C608" t="s">
+        <v>2018</v>
+      </c>
+      <c r="D608" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E608" t="s">
+        <v>16</v>
+      </c>
+      <c r="F608" t="s">
+        <v>1100</v>
+      </c>
+      <c r="G608" t="s">
+        <v>16</v>
+      </c>
+      <c r="H608" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="609" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A609" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B609" t="s">
+        <v>619</v>
+      </c>
+      <c r="C609" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D609" t="s">
+        <v>902</v>
+      </c>
+      <c r="E609" t="s">
+        <v>2021</v>
+      </c>
+      <c r="F609" t="s">
+        <v>902</v>
+      </c>
+      <c r="G609" t="s">
+        <v>2021</v>
+      </c>
+      <c r="H609" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="610" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A610" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B610" t="s">
+        <v>619</v>
+      </c>
+      <c r="C610" t="s">
+        <v>2023</v>
+      </c>
+      <c r="D610" t="s">
+        <v>760</v>
+      </c>
+      <c r="E610" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F610" t="s">
+        <v>760</v>
+      </c>
+      <c r="G610" t="s">
+        <v>1590</v>
+      </c>
+      <c r="H610" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="611" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A611" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B611" t="s">
+        <v>700</v>
+      </c>
+      <c r="C611" t="s">
+        <v>2025</v>
+      </c>
+      <c r="D611" t="s">
+        <v>722</v>
+      </c>
+      <c r="E611" t="s">
+        <v>2026</v>
+      </c>
+      <c r="F611" t="s">
+        <v>722</v>
+      </c>
+      <c r="G611" t="s">
+        <v>2026</v>
+      </c>
+      <c r="H611" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="612" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A612" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B612" t="s">
+        <v>700</v>
+      </c>
+      <c r="C612" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D612" t="s">
+        <v>2029</v>
+      </c>
+      <c r="E612" t="s">
+        <v>2030</v>
+      </c>
+      <c r="F612" t="s">
+        <v>2029</v>
+      </c>
+      <c r="G612" t="s">
+        <v>2030</v>
+      </c>
+      <c r="H612" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="613" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A613" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B613" t="s">
+        <v>700</v>
+      </c>
+      <c r="C613" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D613" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E613" t="s">
+        <v>2034</v>
+      </c>
+      <c r="F613" t="s">
+        <v>2033</v>
+      </c>
+      <c r="G613" t="s">
+        <v>2034</v>
+      </c>
+      <c r="H613" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="614" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A614" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B614" t="s">
+        <v>700</v>
+      </c>
+      <c r="C614" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D614" t="s">
+        <v>407</v>
+      </c>
+      <c r="E614" t="s">
+        <v>2037</v>
+      </c>
+      <c r="F614" t="s">
+        <v>407</v>
+      </c>
+      <c r="G614" t="s">
+        <v>2037</v>
+      </c>
+      <c r="H614" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="615" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A615" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B615" t="s">
+        <v>700</v>
+      </c>
+      <c r="C615" t="s">
+        <v>2039</v>
+      </c>
+      <c r="D615" t="s">
+        <v>2040</v>
+      </c>
+      <c r="E615" t="s">
+        <v>2041</v>
+      </c>
+      <c r="F615" t="s">
+        <v>2040</v>
+      </c>
+      <c r="G615" t="s">
+        <v>2041</v>
+      </c>
+      <c r="H615" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="616" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A616" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B616" t="s">
+        <v>789</v>
+      </c>
+      <c r="C616" t="s">
+        <v>2043</v>
+      </c>
+      <c r="D616" t="s">
+        <v>2044</v>
+      </c>
+      <c r="E616" t="s">
+        <v>2045</v>
+      </c>
+      <c r="F616" t="s">
+        <v>2044</v>
+      </c>
+      <c r="G616" t="s">
+        <v>2045</v>
+      </c>
+      <c r="H616" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="617" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A617" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B617" t="s">
+        <v>789</v>
+      </c>
+      <c r="C617" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D617" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E617" t="s">
+        <v>2049</v>
+      </c>
+      <c r="F617" t="s">
+        <v>2048</v>
+      </c>
+      <c r="G617" t="s">
+        <v>2049</v>
+      </c>
+      <c r="H617" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="618" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A618" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B618" t="s">
+        <v>789</v>
+      </c>
+      <c r="C618" t="s">
+        <v>2051</v>
+      </c>
+      <c r="D618" t="s">
+        <v>706</v>
+      </c>
+      <c r="E618" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F618" t="s">
+        <v>706</v>
+      </c>
+      <c r="G618" t="s">
+        <v>2052</v>
+      </c>
+      <c r="H618" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="619" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A619" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B619" t="s">
+        <v>789</v>
+      </c>
+      <c r="C619" t="s">
+        <v>2054</v>
+      </c>
+      <c r="D619" t="s">
+        <v>2055</v>
+      </c>
+      <c r="E619" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F619" t="s">
+        <v>2055</v>
+      </c>
+      <c r="G619" t="s">
+        <v>2057</v>
+      </c>
+      <c r="H619" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="620" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A620" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B620" t="s">
+        <v>789</v>
+      </c>
+      <c r="C620" t="s">
+        <v>2059</v>
+      </c>
+      <c r="D620" t="s">
+        <v>2060</v>
+      </c>
+      <c r="E620" t="s">
+        <v>2061</v>
+      </c>
+      <c r="F620" t="s">
+        <v>2060</v>
+      </c>
+      <c r="G620" t="s">
+        <v>2061</v>
+      </c>
+      <c r="H620" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="621" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A621" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B621" t="s">
+        <v>849</v>
+      </c>
+      <c r="C621" t="s">
+        <v>2063</v>
+      </c>
+      <c r="D621" t="s">
+        <v>302</v>
+      </c>
+      <c r="E621" t="s">
+        <v>2064</v>
+      </c>
+      <c r="F621" t="s">
+        <v>302</v>
+      </c>
+      <c r="G621" t="s">
+        <v>2064</v>
+      </c>
+      <c r="H621" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="622" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A622" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B622" t="s">
+        <v>849</v>
+      </c>
+      <c r="C622" t="s">
+        <v>2066</v>
+      </c>
+      <c r="D622" t="s">
+        <v>260</v>
+      </c>
+      <c r="E622" t="s">
+        <v>2067</v>
+      </c>
+      <c r="F622" t="s">
+        <v>260</v>
+      </c>
+      <c r="G622" t="s">
+        <v>2067</v>
+      </c>
+      <c r="H622" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="623" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A623" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B623" t="s">
+        <v>939</v>
+      </c>
+      <c r="C623" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D623" t="s">
+        <v>2070</v>
+      </c>
+      <c r="E623" t="s">
+        <v>2071</v>
+      </c>
+      <c r="F623" t="s">
+        <v>2072</v>
+      </c>
+      <c r="G623" t="s">
+        <v>2071</v>
+      </c>
+      <c r="H623" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="624" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A624" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B624" t="s">
+        <v>939</v>
+      </c>
+      <c r="C624" t="s">
+        <v>2074</v>
+      </c>
+      <c r="D624" t="s">
+        <v>2075</v>
+      </c>
+      <c r="E624" t="s">
+        <v>2076</v>
+      </c>
+      <c r="F624" t="s">
+        <v>2075</v>
+      </c>
+      <c r="G624" t="s">
+        <v>2076</v>
+      </c>
+      <c r="H624" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="625" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A625" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B625" t="s">
+        <v>939</v>
+      </c>
+      <c r="C625" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D625" t="s">
+        <v>2079</v>
+      </c>
+      <c r="E625" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F625" t="s">
+        <v>2079</v>
+      </c>
+      <c r="G625" t="s">
+        <v>1590</v>
+      </c>
+      <c r="H625" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="626" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B626" t="s">
+        <v>939</v>
+      </c>
+      <c r="C626" t="s">
+        <v>2081</v>
+      </c>
+      <c r="D626" t="s">
+        <v>1646</v>
+      </c>
+      <c r="E626" t="s">
+        <v>2082</v>
+      </c>
+      <c r="F626" t="s">
+        <v>1646</v>
+      </c>
+      <c r="G626" t="s">
+        <v>2082</v>
+      </c>
+      <c r="H626" t="s">
+        <v>2083</v>
+      </c>
+    </row>
+    <row r="627" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A627" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B627" t="s">
+        <v>939</v>
+      </c>
+      <c r="C627" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D627" t="s">
+        <v>158</v>
+      </c>
+      <c r="E627" t="s">
+        <v>2085</v>
+      </c>
+      <c r="F627" t="s">
+        <v>158</v>
+      </c>
+      <c r="G627" t="s">
+        <v>2085</v>
+      </c>
+      <c r="H627" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="628" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B628" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C628" t="s">
+        <v>2087</v>
+      </c>
+      <c r="D628" t="s">
+        <v>183</v>
+      </c>
+      <c r="E628" t="s">
+        <v>2088</v>
+      </c>
+      <c r="F628" t="s">
+        <v>183</v>
+      </c>
+      <c r="G628" t="s">
+        <v>2088</v>
+      </c>
+      <c r="H628" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="629" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B629" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C629" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D629" t="s">
+        <v>321</v>
+      </c>
+      <c r="E629" t="s">
+        <v>2091</v>
+      </c>
+      <c r="F629" t="s">
+        <v>321</v>
+      </c>
+      <c r="G629" t="s">
+        <v>2091</v>
+      </c>
+      <c r="H629" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="630" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B630" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C630" t="s">
+        <v>2093</v>
+      </c>
+      <c r="D630" t="s">
+        <v>118</v>
+      </c>
+      <c r="E630" t="s">
+        <v>655</v>
+      </c>
+      <c r="F630" t="s">
+        <v>118</v>
+      </c>
+      <c r="G630" t="s">
+        <v>655</v>
+      </c>
+      <c r="H630" t="s">
+        <v>2094</v>
+      </c>
+    </row>
+    <row r="631" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A631" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B631" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C631" t="s">
+        <v>2095</v>
+      </c>
+      <c r="D631" t="s">
+        <v>2096</v>
+      </c>
+      <c r="E631" t="s">
+        <v>2097</v>
+      </c>
+      <c r="F631" t="s">
+        <v>2096</v>
+      </c>
+      <c r="G631" t="s">
+        <v>2097</v>
+      </c>
+      <c r="H631" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="632" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A632" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B632" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C632" t="s">
+        <v>2099</v>
+      </c>
+      <c r="D632" t="s">
+        <v>2100</v>
+      </c>
+      <c r="E632" t="s">
+        <v>2101</v>
+      </c>
+      <c r="F632" t="s">
+        <v>2100</v>
+      </c>
+      <c r="G632" t="s">
+        <v>2101</v>
+      </c>
+      <c r="H632" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="633" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A633" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B633" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C633" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D633" t="s">
+        <v>379</v>
+      </c>
+      <c r="E633" t="s">
+        <v>2104</v>
+      </c>
+      <c r="F633" t="s">
+        <v>379</v>
+      </c>
+      <c r="G633" t="s">
+        <v>2104</v>
+      </c>
+      <c r="H633" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="634" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A634" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B634" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C634" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D634" t="s">
+        <v>2107</v>
+      </c>
+      <c r="E634" t="s">
+        <v>2108</v>
+      </c>
+      <c r="F634" t="s">
+        <v>2107</v>
+      </c>
+      <c r="G634" t="s">
+        <v>2108</v>
+      </c>
+      <c r="H634" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="635" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A635" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B635" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C635" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D635" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E635" t="s">
+        <v>2111</v>
+      </c>
+      <c r="F635" t="s">
+        <v>1219</v>
+      </c>
+      <c r="G635" t="s">
+        <v>2111</v>
+      </c>
+      <c r="H635" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="636" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B636" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C636" t="s">
+        <v>2113</v>
+      </c>
+      <c r="D636" t="s">
+        <v>706</v>
+      </c>
+      <c r="E636" t="s">
+        <v>253</v>
+      </c>
+      <c r="F636" t="s">
+        <v>706</v>
+      </c>
+      <c r="G636" t="s">
+        <v>253</v>
+      </c>
+      <c r="H636" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="637" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A637" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B637" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C637" t="s">
+        <v>2115</v>
+      </c>
+      <c r="D637" t="s">
+        <v>90</v>
+      </c>
+      <c r="E637" t="s">
+        <v>2116</v>
+      </c>
+      <c r="F637" t="s">
+        <v>90</v>
+      </c>
+      <c r="G637" t="s">
+        <v>2116</v>
+      </c>
+      <c r="H637" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="638" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B638" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C638" t="s">
+        <v>2118</v>
+      </c>
+      <c r="D638" t="s">
+        <v>2119</v>
+      </c>
+      <c r="E638" t="s">
+        <v>2120</v>
+      </c>
+      <c r="F638" t="s">
+        <v>2119</v>
+      </c>
+      <c r="G638" t="s">
+        <v>2120</v>
+      </c>
+      <c r="H638" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="639" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B639" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C639" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D639" t="s">
+        <v>2123</v>
+      </c>
+      <c r="E639" t="s">
+        <v>2124</v>
+      </c>
+      <c r="F639" t="s">
+        <v>2123</v>
+      </c>
+      <c r="G639" t="s">
+        <v>2124</v>
+      </c>
+      <c r="H639" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="640" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B640" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C640" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D640" t="s">
+        <v>2127</v>
+      </c>
+      <c r="E640" t="s">
+        <v>540</v>
+      </c>
+      <c r="F640" t="s">
+        <v>2127</v>
+      </c>
+      <c r="G640" t="s">
+        <v>540</v>
+      </c>
+      <c r="H640" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="641" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B641" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C641" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D641" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E641" t="s">
+        <v>2130</v>
+      </c>
+      <c r="F641" t="s">
+        <v>2015</v>
+      </c>
+      <c r="G641" t="s">
+        <v>2130</v>
+      </c>
+      <c r="H641" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="642" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A642" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B642" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C642" t="s">
+        <v>2132</v>
+      </c>
+      <c r="D642" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E642" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F642" t="s">
+        <v>2133</v>
+      </c>
+      <c r="G642" t="s">
+        <v>2134</v>
+      </c>
+      <c r="H642" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="643" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A643" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B643" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C643" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D643" t="s">
+        <v>747</v>
+      </c>
+      <c r="E643" t="s">
+        <v>2137</v>
+      </c>
+      <c r="F643" t="s">
+        <v>747</v>
+      </c>
+      <c r="G643" t="s">
+        <v>2137</v>
+      </c>
+      <c r="H643" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="644" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A644" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B644" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C644" t="s">
+        <v>2139</v>
+      </c>
+      <c r="D644" t="s">
+        <v>2140</v>
+      </c>
+      <c r="E644" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F644" t="s">
+        <v>2140</v>
+      </c>
+      <c r="G644" t="s">
+        <v>2141</v>
+      </c>
+      <c r="H644" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="645" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A645" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B645" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C645" t="s">
+        <v>2143</v>
+      </c>
+      <c r="D645" t="s">
+        <v>2144</v>
+      </c>
+      <c r="E645" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F645" t="s">
+        <v>2144</v>
+      </c>
+      <c r="G645" t="s">
+        <v>2146</v>
+      </c>
+      <c r="H645" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="646" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A646" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B646" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C646" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D646" t="s">
+        <v>28</v>
+      </c>
+      <c r="E646" t="s">
+        <v>2149</v>
+      </c>
+      <c r="F646" t="s">
+        <v>28</v>
+      </c>
+      <c r="G646" t="s">
+        <v>2149</v>
+      </c>
+      <c r="H646" t="s">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="647" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A647" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B647" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C647" t="s">
+        <v>2151</v>
+      </c>
+      <c r="D647" t="s">
+        <v>49</v>
+      </c>
+      <c r="E647" t="s">
+        <v>2152</v>
+      </c>
+      <c r="F647" t="s">
+        <v>49</v>
+      </c>
+      <c r="G647" t="s">
+        <v>2152</v>
+      </c>
+      <c r="H647" t="s">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="648" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A648" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B648" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C648" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D648" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E648" t="s">
+        <v>1366</v>
+      </c>
+      <c r="F648" t="s">
+        <v>2155</v>
+      </c>
+      <c r="G648" t="s">
+        <v>1366</v>
+      </c>
+      <c r="H648" t="s">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="649" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A649" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B649" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C649" t="s">
+        <v>2157</v>
+      </c>
+      <c r="D649" t="s">
+        <v>600</v>
+      </c>
+      <c r="E649" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F649" t="s">
+        <v>600</v>
+      </c>
+      <c r="G649" t="s">
+        <v>1319</v>
+      </c>
+      <c r="H649" t="s">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="650" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A650" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B650" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C650" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D650" t="s">
+        <v>906</v>
+      </c>
+      <c r="E650" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F650" t="s">
+        <v>906</v>
+      </c>
+      <c r="G650" t="s">
+        <v>2160</v>
+      </c>
+      <c r="H650" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="651" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A651" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B651" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C651" t="s">
+        <v>2162</v>
+      </c>
+      <c r="D651" t="s">
+        <v>379</v>
+      </c>
+      <c r="E651" t="s">
+        <v>2163</v>
+      </c>
+      <c r="F651" t="s">
+        <v>379</v>
+      </c>
+      <c r="G651" t="s">
+        <v>2163</v>
+      </c>
+      <c r="H651" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="652" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A652" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B652" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C652" t="s">
+        <v>2165</v>
+      </c>
+      <c r="D652" t="s">
+        <v>2166</v>
+      </c>
+      <c r="E652" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F652" t="s">
+        <v>2168</v>
+      </c>
+      <c r="G652" t="s">
+        <v>2169</v>
+      </c>
+      <c r="H652" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="653" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A653" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B653" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C653" t="s">
+        <v>2171</v>
+      </c>
+      <c r="D653" t="s">
+        <v>2172</v>
+      </c>
+      <c r="E653" t="s">
+        <v>2173</v>
+      </c>
+      <c r="F653" t="s">
+        <v>2172</v>
+      </c>
+      <c r="G653" t="s">
+        <v>2173</v>
+      </c>
+      <c r="H653" t="s">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="654" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A654" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B654" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C654" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D654" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E654" t="s">
+        <v>1366</v>
+      </c>
+      <c r="F654" t="s">
+        <v>2155</v>
+      </c>
+      <c r="G654" t="s">
+        <v>1366</v>
+      </c>
+      <c r="H654" t="s">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="655" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A655" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B655" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C655" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D655" t="s">
+        <v>906</v>
+      </c>
+      <c r="E655" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F655" t="s">
+        <v>906</v>
+      </c>
+      <c r="G655" t="s">
+        <v>2160</v>
+      </c>
+      <c r="H655" t="s">
+        <v>2161</v>
+      </c>
+    </row>
+    <row r="656" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A656" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B656" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C656" t="s">
+        <v>1584</v>
+      </c>
+      <c r="D656" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E656" t="s">
+        <v>1586</v>
+      </c>
+      <c r="F656" t="s">
+        <v>1585</v>
+      </c>
+      <c r="G656" t="s">
+        <v>1586</v>
+      </c>
+      <c r="H656" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="657" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A657" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B657" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C657" t="s">
+        <v>2175</v>
+      </c>
+      <c r="D657" t="s">
+        <v>810</v>
+      </c>
+      <c r="E657" t="s">
+        <v>2176</v>
+      </c>
+      <c r="F657" t="s">
+        <v>810</v>
+      </c>
+      <c r="G657" t="s">
+        <v>2176</v>
+      </c>
+      <c r="H657" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="658" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A658" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B658" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C658" t="s">
+        <v>2178</v>
+      </c>
+      <c r="D658" t="s">
+        <v>131</v>
+      </c>
+      <c r="E658" t="s">
+        <v>2179</v>
+      </c>
+      <c r="F658" t="s">
+        <v>131</v>
+      </c>
+      <c r="G658" t="s">
+        <v>2179</v>
+      </c>
+      <c r="H658" t="s">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="659" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A659" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B659" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C659" t="s">
+        <v>2178</v>
+      </c>
+      <c r="D659" t="s">
+        <v>131</v>
+      </c>
+      <c r="E659" t="s">
+        <v>2179</v>
+      </c>
+      <c r="F659" t="s">
+        <v>131</v>
+      </c>
+      <c r="G659" t="s">
+        <v>2179</v>
+      </c>
+      <c r="H659" t="s">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="660" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A660" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B660" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C660" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D660" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E660" t="s">
+        <v>2182</v>
+      </c>
+      <c r="F660" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G660" t="s">
+        <v>2182</v>
+      </c>
+      <c r="H660" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="661" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A661" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B661" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C661" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D661" t="s">
+        <v>775</v>
+      </c>
+      <c r="E661" t="s">
+        <v>2185</v>
+      </c>
+      <c r="F661" t="s">
+        <v>775</v>
+      </c>
+      <c r="G661" t="s">
+        <v>2186</v>
+      </c>
+      <c r="H661" t="s">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="662" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A662" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B662" t="s">
+        <v>1628</v>
+      </c>
+      <c r="C662" t="s">
+        <v>2175</v>
+      </c>
+      <c r="D662" t="s">
+        <v>810</v>
+      </c>
+      <c r="E662" t="s">
+        <v>2176</v>
+      </c>
+      <c r="F662" t="s">
+        <v>810</v>
+      </c>
+      <c r="G662" t="s">
+        <v>2176</v>
+      </c>
+      <c r="H662" t="s">
+        <v>2177</v>
+      </c>
+    </row>
+    <row r="663" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A663" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B663" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C663" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D663" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E663" t="s">
+        <v>2182</v>
+      </c>
+      <c r="F663" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G663" t="s">
+        <v>2182</v>
+      </c>
+      <c r="H663" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="664" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A664" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B664" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C664" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D664" t="s">
+        <v>775</v>
+      </c>
+      <c r="E664" t="s">
+        <v>2185</v>
+      </c>
+      <c r="F664" t="s">
+        <v>775</v>
+      </c>
+      <c r="G664" t="s">
+        <v>2186</v>
+      </c>
+      <c r="H664" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="665" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A665" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B665" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C665" t="s">
+        <v>2189</v>
+      </c>
+      <c r="D665" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E665" t="s">
+        <v>2191</v>
+      </c>
+      <c r="F665" t="s">
+        <v>2190</v>
+      </c>
+      <c r="G665" t="s">
+        <v>2191</v>
+      </c>
+      <c r="H665" t="s">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="666" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A666" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B666" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C666" t="s">
+        <v>2193</v>
+      </c>
+      <c r="D666" t="s">
+        <v>1838</v>
+      </c>
+      <c r="E666" t="s">
+        <v>2194</v>
+      </c>
+      <c r="F666" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G666" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H666" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="667" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A667" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B667" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C667" t="s">
+        <v>2196</v>
+      </c>
+      <c r="D667" t="s">
+        <v>438</v>
+      </c>
+      <c r="E667" t="s">
+        <v>2197</v>
+      </c>
+      <c r="F667" t="s">
+        <v>438</v>
+      </c>
+      <c r="G667" t="s">
+        <v>2197</v>
+      </c>
+      <c r="H667" t="s">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="668" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A668" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B668" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C668" t="s">
+        <v>2199</v>
+      </c>
+      <c r="D668" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E668" t="s">
+        <v>2200</v>
+      </c>
+      <c r="F668" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G668" t="s">
+        <v>2200</v>
+      </c>
+      <c r="H668" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="669" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A669" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B669" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C669" t="s">
+        <v>2202</v>
+      </c>
+      <c r="D669" t="s">
+        <v>2203</v>
+      </c>
+      <c r="E669" t="s">
+        <v>2204</v>
+      </c>
+      <c r="F669" t="s">
+        <v>2203</v>
+      </c>
+      <c r="G669" t="s">
+        <v>2204</v>
+      </c>
+      <c r="H669" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="670" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A670" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B670" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C670" t="s">
+        <v>2189</v>
+      </c>
+      <c r="D670" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E670" t="s">
+        <v>2191</v>
+      </c>
+      <c r="F670" t="s">
+        <v>2190</v>
+      </c>
+      <c r="G670" t="s">
+        <v>2191</v>
+      </c>
+      <c r="H670" t="s">
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="671" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A671" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B671" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C671" t="s">
+        <v>2193</v>
+      </c>
+      <c r="D671" t="s">
+        <v>1838</v>
+      </c>
+      <c r="E671" t="s">
+        <v>2194</v>
+      </c>
+      <c r="F671" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G671" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H671" t="s">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="672" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A672" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B672" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C672" t="s">
+        <v>2196</v>
+      </c>
+      <c r="D672" t="s">
+        <v>438</v>
+      </c>
+      <c r="E672" t="s">
+        <v>2197</v>
+      </c>
+      <c r="F672" t="s">
+        <v>438</v>
+      </c>
+      <c r="G672" t="s">
+        <v>2197</v>
+      </c>
+      <c r="H672" t="s">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="673" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A673" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B673" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C673" t="s">
+        <v>2206</v>
+      </c>
+      <c r="D673" t="s">
+        <v>2207</v>
+      </c>
+      <c r="E673" t="s">
+        <v>2208</v>
+      </c>
+      <c r="F673" t="s">
+        <v>2207</v>
+      </c>
+      <c r="G673" t="s">
+        <v>2208</v>
+      </c>
+      <c r="H673" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="674" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A674" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B674" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C674" t="s">
+        <v>2210</v>
+      </c>
+      <c r="D674" t="s">
+        <v>697</v>
+      </c>
+      <c r="E674" t="s">
+        <v>2211</v>
+      </c>
+      <c r="F674" t="s">
+        <v>697</v>
+      </c>
+      <c r="G674" t="s">
+        <v>2211</v>
+      </c>
+      <c r="H674" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="675" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A675" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B675" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C675" t="s">
+        <v>2199</v>
+      </c>
+      <c r="D675" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E675" t="s">
+        <v>2200</v>
+      </c>
+      <c r="F675" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G675" t="s">
+        <v>2200</v>
+      </c>
+      <c r="H675" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="676" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A676" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B676" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C676" t="s">
+        <v>2213</v>
+      </c>
+      <c r="D676" t="s">
+        <v>806</v>
+      </c>
+      <c r="E676" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F676" t="s">
+        <v>806</v>
+      </c>
+      <c r="G676" t="s">
+        <v>2214</v>
+      </c>
+      <c r="H676" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="677" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A677" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B677" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C677" t="s">
+        <v>2216</v>
+      </c>
+      <c r="D677" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E677" t="s">
+        <v>2217</v>
+      </c>
+      <c r="F677" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G677" t="s">
+        <v>2217</v>
+      </c>
+      <c r="H677" t="s">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="678" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A678" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B678" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C678" t="s">
+        <v>2219</v>
+      </c>
+      <c r="D678" t="s">
+        <v>764</v>
+      </c>
+      <c r="E678" t="s">
+        <v>2220</v>
+      </c>
+      <c r="F678" t="s">
+        <v>764</v>
+      </c>
+      <c r="G678" t="s">
+        <v>2220</v>
+      </c>
+      <c r="H678" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="679" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A679" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B679" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C679" t="s">
+        <v>2222</v>
+      </c>
+      <c r="D679" t="s">
+        <v>379</v>
+      </c>
+      <c r="E679" t="s">
+        <v>988</v>
+      </c>
+      <c r="F679" t="s">
+        <v>379</v>
+      </c>
+      <c r="G679" t="s">
+        <v>988</v>
+      </c>
+      <c r="H679" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="680" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A680" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B680" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C680" t="s">
+        <v>2224</v>
+      </c>
+      <c r="D680" t="s">
+        <v>544</v>
+      </c>
+      <c r="E680" t="s">
+        <v>2225</v>
+      </c>
+      <c r="F680" t="s">
+        <v>544</v>
+      </c>
+      <c r="G680" t="s">
+        <v>2225</v>
+      </c>
+      <c r="H680" t="s">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="681" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A681" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B681" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C681" t="s">
+        <v>2227</v>
+      </c>
+      <c r="D681" t="s">
+        <v>2228</v>
+      </c>
+      <c r="E681" t="s">
+        <v>2229</v>
+      </c>
+      <c r="F681" t="s">
+        <v>2228</v>
+      </c>
+      <c r="G681" t="s">
+        <v>2229</v>
+      </c>
+      <c r="H681" t="s">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="682" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A682" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B682" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C682" t="s">
+        <v>2231</v>
+      </c>
+      <c r="D682" t="s">
+        <v>564</v>
+      </c>
+      <c r="E682" t="s">
+        <v>2232</v>
+      </c>
+      <c r="F682" t="s">
+        <v>564</v>
+      </c>
+      <c r="G682" t="s">
+        <v>2232</v>
+      </c>
+      <c r="H682" t="s">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="683" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A683" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B683" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C683" t="s">
+        <v>2213</v>
+      </c>
+      <c r="D683" t="s">
+        <v>806</v>
+      </c>
+      <c r="E683" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F683" t="s">
+        <v>806</v>
+      </c>
+      <c r="G683" t="s">
+        <v>2214</v>
+      </c>
+      <c r="H683" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="684" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A684" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B684" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C684" t="s">
+        <v>2202</v>
+      </c>
+      <c r="D684" t="s">
+        <v>2203</v>
+      </c>
+      <c r="E684" t="s">
+        <v>2204</v>
+      </c>
+      <c r="F684" t="s">
+        <v>2203</v>
+      </c>
+      <c r="G684" t="s">
+        <v>2204</v>
+      </c>
+      <c r="H684" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="685" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A685" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B685" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C685" t="s">
+        <v>2234</v>
+      </c>
+      <c r="D685" t="s">
+        <v>810</v>
+      </c>
+      <c r="E685" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F685" t="s">
+        <v>810</v>
+      </c>
+      <c r="G685" t="s">
+        <v>2235</v>
+      </c>
+      <c r="H685" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="686" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A686" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B686" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C686" t="s">
+        <v>2237</v>
+      </c>
+      <c r="D686" t="s">
+        <v>2238</v>
+      </c>
+      <c r="E686" t="s">
+        <v>2239</v>
+      </c>
+      <c r="F686" t="s">
+        <v>2238</v>
+      </c>
+      <c r="G686" t="s">
+        <v>2239</v>
+      </c>
+      <c r="H686" t="s">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="687" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A687" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B687" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C687" t="s">
+        <v>2241</v>
+      </c>
+      <c r="D687" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E687" t="s">
+        <v>16</v>
+      </c>
+      <c r="F687" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G687" t="s">
+        <v>16</v>
+      </c>
+      <c r="H687" t="s">
+        <v>2242</v>
+      </c>
+    </row>
+    <row r="688" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A688" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B688" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C688" t="s">
+        <v>2243</v>
+      </c>
+      <c r="D688" t="s">
+        <v>1852</v>
+      </c>
+      <c r="E688" t="s">
+        <v>2244</v>
+      </c>
+      <c r="F688" t="s">
+        <v>1852</v>
+      </c>
+      <c r="G688" t="s">
+        <v>2244</v>
+      </c>
+      <c r="H688" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="689" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A689" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B689" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C689" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D689" t="s">
+        <v>854</v>
+      </c>
+      <c r="E689" t="s">
+        <v>1758</v>
+      </c>
+      <c r="F689" t="s">
+        <v>854</v>
+      </c>
+      <c r="G689" t="s">
+        <v>1758</v>
+      </c>
+      <c r="H689" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="690" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A690" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B690" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C690" t="s">
+        <v>2246</v>
+      </c>
+      <c r="D690" t="s">
+        <v>2247</v>
+      </c>
+      <c r="E690" t="s">
+        <v>2248</v>
+      </c>
+      <c r="F690" t="s">
+        <v>2247</v>
+      </c>
+      <c r="G690" t="s">
+        <v>2248</v>
+      </c>
+      <c r="H690" t="s">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="691" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A691" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B691" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C691" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D691" t="s">
+        <v>2251</v>
+      </c>
+      <c r="E691" t="s">
+        <v>2252</v>
+      </c>
+      <c r="F691" t="s">
+        <v>2251</v>
+      </c>
+      <c r="G691" t="s">
+        <v>2252</v>
+      </c>
+      <c r="H691" t="s">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="692" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A692" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B692" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C692" t="s">
+        <v>2254</v>
+      </c>
+      <c r="D692" t="s">
+        <v>2255</v>
+      </c>
+      <c r="E692" t="s">
+        <v>2256</v>
+      </c>
+      <c r="F692" t="s">
+        <v>2255</v>
+      </c>
+      <c r="G692" t="s">
+        <v>2256</v>
+      </c>
+      <c r="H692" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="693" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B693" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C693" t="s">
+        <v>2258</v>
+      </c>
+      <c r="D693" t="s">
+        <v>2259</v>
+      </c>
+      <c r="E693" t="s">
+        <v>2260</v>
+      </c>
+      <c r="F693" t="s">
+        <v>2259</v>
+      </c>
+      <c r="G693" t="s">
+        <v>2260</v>
+      </c>
+      <c r="H693" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="694" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A694" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B694" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C694" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D694" t="s">
+        <v>2263</v>
+      </c>
+      <c r="E694" t="s">
+        <v>2264</v>
+      </c>
+      <c r="F694" t="s">
+        <v>2263</v>
+      </c>
+      <c r="G694" t="s">
+        <v>2265</v>
+      </c>
+      <c r="H694" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="695" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A695" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B695" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C695" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D695" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E695" t="s">
+        <v>2268</v>
+      </c>
+      <c r="F695" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G695" t="s">
+        <v>2268</v>
+      </c>
+      <c r="H695" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="696" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A696" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B696" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C696" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D696" t="s">
+        <v>2247</v>
+      </c>
+      <c r="E696" t="s">
+        <v>2271</v>
+      </c>
+      <c r="F696" t="s">
+        <v>2247</v>
+      </c>
+      <c r="G696" t="s">
+        <v>2271</v>
+      </c>
+      <c r="H696" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="697" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A697" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B697" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C697" t="s">
+        <v>2219</v>
+      </c>
+      <c r="D697" t="s">
+        <v>764</v>
+      </c>
+      <c r="E697" t="s">
+        <v>2220</v>
+      </c>
+      <c r="F697" t="s">
+        <v>764</v>
+      </c>
+      <c r="G697" t="s">
+        <v>2220</v>
+      </c>
+      <c r="H697" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="698" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A698" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B698" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C698" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D698" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E698" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F698" t="s">
+        <v>1761</v>
+      </c>
+      <c r="G698" t="s">
+        <v>1762</v>
+      </c>
+      <c r="H698" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="699" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A699" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B699" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C699" t="s">
+        <v>2273</v>
+      </c>
+      <c r="D699" t="s">
+        <v>430</v>
+      </c>
+      <c r="E699" t="s">
+        <v>2274</v>
+      </c>
+      <c r="F699" t="s">
+        <v>430</v>
+      </c>
+      <c r="G699" t="s">
+        <v>2274</v>
+      </c>
+      <c r="H699" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="700" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A700" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B700" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C700" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D700" t="s">
+        <v>540</v>
+      </c>
+      <c r="E700" t="s">
+        <v>2277</v>
+      </c>
+      <c r="F700" t="s">
+        <v>540</v>
+      </c>
+      <c r="G700" t="s">
+        <v>2277</v>
+      </c>
+      <c r="H700" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="701" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A701" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B701" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C701" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D701" t="s">
+        <v>516</v>
+      </c>
+      <c r="E701" t="s">
+        <v>383</v>
+      </c>
+      <c r="F701" t="s">
+        <v>516</v>
+      </c>
+      <c r="G701" t="s">
+        <v>383</v>
+      </c>
+      <c r="H701" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="702" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A702" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B702" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C702" t="s">
+        <v>2279</v>
+      </c>
+      <c r="D702" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E702" t="s">
+        <v>2280</v>
+      </c>
+      <c r="F702" t="s">
+        <v>1063</v>
+      </c>
+      <c r="G702" t="s">
+        <v>2280</v>
+      </c>
+      <c r="H702" t="s">
+        <v>2281</v>
+      </c>
+    </row>
+    <row r="703" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A703" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B703" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C703" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D703" t="s">
+        <v>1793</v>
+      </c>
+      <c r="E703" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F703" t="s">
+        <v>1793</v>
+      </c>
+      <c r="G703" t="s">
+        <v>1795</v>
+      </c>
+      <c r="H703" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="704" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A704" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B704" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C704" t="s">
+        <v>2282</v>
+      </c>
+      <c r="D704" t="s">
+        <v>2283</v>
+      </c>
+      <c r="E704" t="s">
+        <v>2284</v>
+      </c>
+      <c r="F704" t="s">
+        <v>2283</v>
+      </c>
+      <c r="G704" t="s">
+        <v>2285</v>
+      </c>
+      <c r="H704" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="705" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A705" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B705" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C705" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D705" t="s">
+        <v>2288</v>
+      </c>
+      <c r="E705" t="s">
+        <v>2289</v>
+      </c>
+      <c r="F705" t="s">
+        <v>2288</v>
+      </c>
+      <c r="G705" t="s">
+        <v>2289</v>
+      </c>
+      <c r="H705" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="706" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A706" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B706" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C706" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D706" t="s">
+        <v>846</v>
+      </c>
+      <c r="E706" t="s">
+        <v>2292</v>
+      </c>
+      <c r="F706" t="s">
+        <v>846</v>
+      </c>
+      <c r="G706" t="s">
+        <v>2292</v>
+      </c>
+      <c r="H706" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="707" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A707" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B707" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C707" t="s">
+        <v>2294</v>
+      </c>
+      <c r="D707" t="s">
+        <v>72</v>
+      </c>
+      <c r="E707" t="s">
+        <v>2295</v>
+      </c>
+      <c r="F707" t="s">
+        <v>72</v>
+      </c>
+      <c r="G707" t="s">
+        <v>2295</v>
+      </c>
+      <c r="H707" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+    <row r="708" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A708" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B708" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C708" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D708" t="s">
+        <v>2298</v>
+      </c>
+      <c r="E708" t="s">
+        <v>2299</v>
+      </c>
+      <c r="F708" t="s">
+        <v>2298</v>
+      </c>
+      <c r="G708" t="s">
+        <v>2299</v>
+      </c>
+      <c r="H708" t="s">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="709" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A709" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B709" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C709" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D709" t="s">
+        <v>902</v>
+      </c>
+      <c r="E709" t="s">
+        <v>2302</v>
+      </c>
+      <c r="F709" t="s">
+        <v>902</v>
+      </c>
+      <c r="G709" t="s">
+        <v>2302</v>
+      </c>
+      <c r="H709" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="710" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A710" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B710" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C710" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D710" t="s">
+        <v>902</v>
+      </c>
+      <c r="E710" t="s">
+        <v>317</v>
+      </c>
+      <c r="F710" t="s">
+        <v>902</v>
+      </c>
+      <c r="G710" t="s">
+        <v>317</v>
+      </c>
+      <c r="H710" t="s">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="711" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A711" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B711" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C711" t="s">
+        <v>2222</v>
+      </c>
+      <c r="D711" t="s">
+        <v>379</v>
+      </c>
+      <c r="E711" t="s">
+        <v>988</v>
+      </c>
+      <c r="F711" t="s">
+        <v>379</v>
+      </c>
+      <c r="G711" t="s">
+        <v>988</v>
+      </c>
+      <c r="H711" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="712" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A712" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B712" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C712" t="s">
+        <v>2306</v>
+      </c>
+      <c r="D712" t="s">
+        <v>72</v>
+      </c>
+      <c r="E712" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F712" t="s">
+        <v>72</v>
+      </c>
+      <c r="G712" t="s">
+        <v>2307</v>
+      </c>
+      <c r="H712" t="s">
+        <v>2308</v>
+      </c>
+    </row>
+    <row r="713" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A713" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B713" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C713" t="s">
+        <v>2309</v>
+      </c>
+      <c r="D713" t="s">
+        <v>654</v>
+      </c>
+      <c r="E713" t="s">
+        <v>2310</v>
+      </c>
+      <c r="F713" t="s">
+        <v>654</v>
+      </c>
+      <c r="G713" t="s">
+        <v>2310</v>
+      </c>
+      <c r="H713" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="714" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A714" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B714" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C714" t="s">
+        <v>2312</v>
+      </c>
+      <c r="D714" t="s">
+        <v>167</v>
+      </c>
+      <c r="E714" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F714" t="s">
+        <v>167</v>
+      </c>
+      <c r="G714" t="s">
+        <v>1600</v>
+      </c>
+      <c r="H714" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="715" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A715" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B715" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C715" t="s">
+        <v>2314</v>
+      </c>
+      <c r="D715" t="s">
+        <v>414</v>
+      </c>
+      <c r="E715" t="s">
+        <v>2315</v>
+      </c>
+      <c r="F715" t="s">
+        <v>414</v>
+      </c>
+      <c r="G715" t="s">
+        <v>2315</v>
+      </c>
+      <c r="H715" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="716" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A716" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B716" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C716" t="s">
+        <v>2317</v>
+      </c>
+      <c r="D716" t="s">
+        <v>540</v>
+      </c>
+      <c r="E716" t="s">
+        <v>2318</v>
+      </c>
+      <c r="F716" t="s">
+        <v>540</v>
+      </c>
+      <c r="G716" t="s">
+        <v>2318</v>
+      </c>
+      <c r="H716" t="s">
+        <v>2319</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>